<commit_message>
improved external workbook mapping in formula
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/externals/external01.xlsx
+++ b/t/regression/xlsx_files/externals/external01.xlsx
@@ -4,14 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="16515" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="1485" yWindow="1965" windowWidth="15510" windowHeight="6180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet With Spaces" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet's &quot;nam({e})!&quot;" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="EXTNAME1">Sheet1!$A$2</definedName>
+    <definedName name="NAMED">'Sheet With Spaces'!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Named</t>
+  </si>
+  <si>
+    <t>BLABLA</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -348,9 +367,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -359,19 +380,55 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>